<commit_message>
add abbreviations tab to spreadsheet
</commit_message>
<xml_diff>
--- a/Facilities De-Dupilcation Query Results.xlsx
+++ b/Facilities De-Dupilcation Query Results.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\DCP\db-facilities-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{708F145D-8C22-4938-9760-AB578B2E8CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C5BC00A5-6AEC-45B0-AED0-E73A6CBF4734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1680" windowWidth="20565" windowHeight="11213"/>
+    <workbookView xWindow="120" yWindow="1680" windowWidth="20565" windowHeight="11213" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="similar_facnames" sheetId="1" r:id="rId1"/>
-    <sheet name="sending_agencies" sheetId="2" r:id="rId2"/>
+    <sheet name="abbreviations" sheetId="3" r:id="rId2"/>
+    <sheet name="sending_agencies" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1806" uniqueCount="465">
   <si>
     <t>id</t>
   </si>
@@ -1284,6 +1285,138 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>INST</t>
+  </si>
+  <si>
+    <t>INSTITUTE</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>CENTER</t>
+  </si>
+  <si>
+    <t>SCH</t>
+  </si>
+  <si>
+    <t>SCHOOL</t>
+  </si>
+  <si>
+    <t>SCH.</t>
+  </si>
+  <si>
+    <t>INC.</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>LLC.</t>
+  </si>
+  <si>
+    <t>LLC</t>
+  </si>
+  <si>
+    <t>DCC</t>
+  </si>
+  <si>
+    <t>DAY CARE CENTER</t>
+  </si>
+  <si>
+    <t>DAYCARE</t>
+  </si>
+  <si>
+    <t>NONMEDICAID</t>
+  </si>
+  <si>
+    <t>NON-MEDICAID</t>
+  </si>
+  <si>
+    <t>NON MEDICAID</t>
+  </si>
+  <si>
+    <t>ECLC</t>
+  </si>
+  <si>
+    <t>EARLY CHILDHOOD CENTER?</t>
+  </si>
+  <si>
+    <t>CORP.</t>
+  </si>
+  <si>
+    <t>CORP</t>
+  </si>
+  <si>
+    <t>KID’S</t>
+  </si>
+  <si>
+    <t>KIDS</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>CHILD CARE CENTER OR DAY CARE CENTER</t>
+  </si>
+  <si>
+    <t>SRVCE</t>
+  </si>
+  <si>
+    <t>SERVICE</t>
+  </si>
+  <si>
+    <t>SER</t>
+  </si>
+  <si>
+    <t>SVS</t>
+  </si>
+  <si>
+    <t>SERVICES</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>STREET</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>ASSOC</t>
+  </si>
+  <si>
+    <t>ASSOCIATION</t>
+  </si>
+  <si>
+    <t>E OR E.</t>
+  </si>
+  <si>
+    <t>EAST</t>
+  </si>
+  <si>
+    <t>W OR W.</t>
+  </si>
+  <si>
+    <t>WEST</t>
+  </si>
+  <si>
+    <t>Seen on table</t>
+  </si>
+  <si>
+    <t>Possible Correction</t>
   </si>
 </sst>
 </file>
@@ -2127,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10846,6 +10979,217 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B1" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B3" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B5" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>428</v>
+      </c>
+      <c r="B6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>430</v>
+      </c>
+      <c r="B7" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>432</v>
+      </c>
+      <c r="B8" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>434</v>
+      </c>
+      <c r="B9" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>435</v>
+      </c>
+      <c r="B10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>437</v>
+      </c>
+      <c r="B11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>438</v>
+      </c>
+      <c r="B12" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>440</v>
+      </c>
+      <c r="B13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>442</v>
+      </c>
+      <c r="B14" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>444</v>
+      </c>
+      <c r="B15" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>446</v>
+      </c>
+      <c r="B16" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>448</v>
+      </c>
+      <c r="B17" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>449</v>
+      </c>
+      <c r="B18" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>451</v>
+      </c>
+      <c r="B19" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>453</v>
+      </c>
+      <c r="B20" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>455</v>
+      </c>
+      <c r="B21" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>457</v>
+      </c>
+      <c r="B22" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>459</v>
+      </c>
+      <c r="B23" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>461</v>
+      </c>
+      <c r="B24" t="s">
+        <v>462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>

</xml_diff>